<commit_message>
Rows transposed to columns in excel files
Standardization of excel files.
</commit_message>
<xml_diff>
--- a/Data/RV1_EUR-CHF average annual exchange rate.xlsx
+++ b/Data/RV1_EUR-CHF average annual exchange rate.xlsx
@@ -428,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -450,145 +450,73 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>1999</v>
+        <v>2008</v>
       </c>
       <c r="B2" s="3">
-        <v>1.6</v>
+        <v>1.59</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>2000</v>
+        <v>2009</v>
       </c>
       <c r="B3" s="3">
-        <v>1.56</v>
+        <v>1.51</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>2001</v>
+        <v>2010</v>
       </c>
       <c r="B4" s="3">
-        <v>1.51</v>
+        <v>1.38</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>2002</v>
+        <v>2011</v>
       </c>
       <c r="B5" s="3">
-        <v>1.47</v>
+        <v>1.23</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>2003</v>
+        <v>2012</v>
       </c>
       <c r="B6" s="3">
-        <v>1.52</v>
+        <v>1.21</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>2004</v>
+        <v>2013</v>
       </c>
       <c r="B7" s="3">
-        <v>1.54</v>
+        <v>1.23</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>2005</v>
+        <v>2014</v>
       </c>
       <c r="B8" s="3">
-        <v>1.55</v>
+        <v>1.21</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>2006</v>
+        <v>2015</v>
       </c>
       <c r="B9" s="3">
-        <v>1.57</v>
+        <v>1.07</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>2007</v>
+        <v>2016</v>
       </c>
       <c r="B10" s="3">
-        <v>1.64</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
-        <v>2008</v>
-      </c>
-      <c r="B11" s="3">
-        <v>1.59</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="1">
-        <v>2009</v>
-      </c>
-      <c r="B12" s="3">
-        <v>1.51</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="1">
-        <v>2010</v>
-      </c>
-      <c r="B13" s="3">
-        <v>1.38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="1">
-        <v>2011</v>
-      </c>
-      <c r="B14" s="3">
-        <v>1.23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="1">
-        <v>2012</v>
-      </c>
-      <c r="B15" s="3">
-        <v>1.21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="1">
-        <v>2013</v>
-      </c>
-      <c r="B16" s="3">
-        <v>1.23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="1">
-        <v>2014</v>
-      </c>
-      <c r="B17" s="3">
-        <v>1.21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="1">
-        <v>2015</v>
-      </c>
-      <c r="B18" s="3">
-        <v>1.07</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="1">
-        <v>2016</v>
-      </c>
-      <c r="B19" s="3">
         <v>1.0900000000000001</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Data Management Module Completed
1. Excel Data in row display necessary for code (excel files closer to
the raw data file);
2. Python module Completed;
3. Exported CSV file for checking results;
4. Tested with different number of excel files and the end result is
robust. It only adds new columns with the new data for the given years
and blank spaces when there is no value.
</commit_message>
<xml_diff>
--- a/Data/RV1_EUR-CHF average annual exchange rate.xlsx
+++ b/Data/RV1_EUR-CHF average annual exchange rate.xlsx
@@ -78,13 +78,13 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -428,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -440,83 +440,67 @@
     <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1">
+        <v>2008</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2009</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2010</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2011</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2012</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2013</v>
+      </c>
+      <c r="H1" s="1">
+        <v>2014</v>
+      </c>
+      <c r="I1" s="1">
+        <v>2015</v>
+      </c>
+      <c r="J1" s="1">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>2008</v>
-      </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
         <v>1.59</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>2009</v>
-      </c>
-      <c r="B3" s="3">
+      <c r="C2" s="2">
         <v>1.51</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>2010</v>
-      </c>
-      <c r="B4" s="3">
+      <c r="D2" s="2">
         <v>1.38</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
-        <v>2011</v>
-      </c>
-      <c r="B5" s="3">
+      <c r="E2" s="2">
         <v>1.23</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
-        <v>2012</v>
-      </c>
-      <c r="B6" s="3">
+      <c r="F2" s="2">
         <v>1.21</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
-        <v>2013</v>
-      </c>
-      <c r="B7" s="3">
+      <c r="G2" s="2">
         <v>1.23</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
-        <v>2014</v>
-      </c>
-      <c r="B8" s="3">
+      <c r="H2" s="2">
         <v>1.21</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
-        <v>2015</v>
-      </c>
-      <c r="B9" s="3">
+      <c r="I2" s="2">
         <v>1.07</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
-        <v>2016</v>
-      </c>
-      <c r="B10" s="3">
+      <c r="J2" s="2">
         <v>1.0900000000000001</v>
       </c>
     </row>

</xml_diff>